<commit_message>
closed slicing for performer
</commit_message>
<xml_diff>
--- a/ExampleIG/output/StructureDefinition-NoVitalSignsObservationBodyHeight.xlsx
+++ b/ExampleIG/output/StructureDefinition-NoVitalSignsObservationBodyHeight.xlsx
@@ -1243,6 +1243,9 @@
 </t>
   </si>
   <si>
+    <t>closed</t>
+  </si>
+  <si>
     <t>Event.performer.actor</t>
   </si>
   <si>
@@ -1293,9 +1296,6 @@
   <si>
     <t xml:space="preserve">type:$this}
 </t>
-  </si>
-  <si>
-    <t>closed</t>
   </si>
   <si>
     <t>ele-1
@@ -8889,7 +8889,7 @@
         <v>82</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>147</v>
+        <v>394</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>388</v>
@@ -8907,19 +8907,19 @@
         <v>171</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="AL54" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="AN54" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="AO54" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="AP54" t="s" s="2">
         <v>82</v>
@@ -8927,13 +8927,13 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B55" t="s" s="2">
         <v>388</v>
       </c>
       <c r="C55" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D55" t="s" s="2">
         <v>82</v>
@@ -8955,7 +8955,7 @@
         <v>94</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="L55" t="s" s="2">
         <v>390</v>
@@ -9031,19 +9031,19 @@
         <v>171</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="AL55" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="AN55" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="AO55" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="AP55" t="s" s="2">
         <v>82</v>
@@ -9051,13 +9051,13 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B56" t="s" s="2">
         <v>388</v>
       </c>
       <c r="C56" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D56" t="s" s="2">
         <v>82</v>
@@ -9079,7 +9079,7 @@
         <v>94</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="L56" t="s" s="2">
         <v>390</v>
@@ -9155,19 +9155,19 @@
         <v>171</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="AN56" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="AO56" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="AP56" t="s" s="2">
         <v>82</v>
@@ -9175,10 +9175,10 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -9201,19 +9201,19 @@
         <v>94</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="O57" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="P57" t="s" s="2">
         <v>82</v>
@@ -9250,17 +9250,17 @@
         <v>82</v>
       </c>
       <c r="AB57" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AC57" s="2"/>
       <c r="AD57" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>80</v>
@@ -9298,7 +9298,7 @@
         <v>416</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C58" t="s" s="2">
         <v>417</v>
@@ -9323,19 +9323,19 @@
         <v>94</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="O58" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="P58" t="s" s="2">
         <v>82</v>
@@ -9384,7 +9384,7 @@
         <v>82</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>80</v>
@@ -13207,7 +13207,7 @@
         <v>628</v>
       </c>
       <c r="O90" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="P90" t="s" s="2">
         <v>82</v>

</xml_diff>